<commit_message>
refactor: improving code structure
</commit_message>
<xml_diff>
--- a/WpfApp2/adresy etykiet DSS test.xlsx
+++ b/WpfApp2/adresy etykiet DSS test.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\profil_arkadiuszw\Desktop\dssmith 2021-01-22\Wpf_Sek20210121\WpfApp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94012806-1527-49E8-BED0-BF7A5930D808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A3AF9-2C33-4829-9C6B-2C462FC6D18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1236" yWindow="3456" windowWidth="17280" windowHeight="8964" xr2:uid="{5AB66045-9732-4E77-868F-C64D3549A316}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{5AB66045-9732-4E77-868F-C64D3549A316}"/>
   </bookViews>
   <sheets>
     <sheet name="lista 1 kolumna" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'lista 1 kolumna'!$A$1:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'lista 1 kolumna'!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -79,6 +79,23 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -92,23 +109,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -126,8 +126,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2B417CB-A6D8-4E3C-97DB-05A27D818CA8}" name="Tabela1" displayName="Tabela1" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{7AD97E40-698E-430D-8E62-DED9B640477A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2B417CB-A6D8-4E3C-97DB-05A27D818CA8}" name="Tabela1" displayName="Tabela1" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{7AD97E40-698E-430D-8E62-DED9B640477A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{89F66763-D8A8-451A-B6C2-0DD14F53F036}" name="@@CTRLSUM@@"/>
     <tableColumn id="2" xr3:uid="{A30F9BFC-E057-4650-A966-6F62EAE8483E}" name="@@SHELF@@"/>
@@ -433,9 +433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995891D9-A103-4FBA-9CC0-A734E78FCC24}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -471,26 +473,74 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  <conditionalFormatting sqref="A2:A10">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4 J2:J4 P2:P4 V2:V4 Y2:Y4 AB2:AB4 AE2:AF4 AI2:AJ4 AM2:AN4 AQ2:AQ4 AS2:AS4 AV2:AV4 AX2:AX4 BA2:BA4 BC2:BC4 BF2:BF4 BH2:BH4 BK2:BK4 BM2:BM4 BP2:BP4 BR2:BR4 BU2:BU4 BW2:BW4 BZ2:BZ4 CB2:CB4 CE2:CE4 CG2:CG4 CJ2:CJ4 CL2:CL4 CO2:CO4 CQ2:CQ4 CT2:CT4 CV2:CV4 CY2:CY4 DA2:DA4 DD2:DD4 DF2:DF4 DH2:DH4 DJ2:DJ4 DL2:DP4">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A4">
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: print script based on appsettings
</commit_message>
<xml_diff>
--- a/WpfApp2/adresy etykiet DSS test.xlsx
+++ b/WpfApp2/adresy etykiet DSS test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\profil_arkadiuszw\Desktop\dssmith 2021-01-22\Wpf_Sek20210121\WpfApp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A3AF9-2C33-4829-9C6B-2C462FC6D18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5371814E-F7C8-4347-A902-538C039D103A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{5AB66045-9732-4E77-868F-C64D3549A316}"/>
+    <workbookView xWindow="2820" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{5AB66045-9732-4E77-868F-C64D3549A316}"/>
   </bookViews>
   <sheets>
     <sheet name="lista 1 kolumna" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>@@CTRLSUM@@</t>
-  </si>
-  <si>
-    <t>@@SHELF@@</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">MHA    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rack    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Coor    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y-Coor    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocType    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CheckSum    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGN1 </t>
+  </si>
+  <si>
+    <t>BP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
   </si>
 </sst>
 </file>
@@ -123,17 +147,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2B417CB-A6D8-4E3C-97DB-05A27D818CA8}" name="Tabela1" displayName="Tabela1" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10" xr:uid="{7AD97E40-698E-430D-8E62-DED9B640477A}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{89F66763-D8A8-451A-B6C2-0DD14F53F036}" name="@@CTRLSUM@@"/>
-    <tableColumn id="2" xr3:uid="{A30F9BFC-E057-4650-A966-6F62EAE8483E}" name="@@SHELF@@"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995891D9-A103-4FBA-9CC0-A734E78FCC24}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,83 +460,95 @@
     <col min="4" max="4" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>11</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>12</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>92</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>12</v>
-      </c>
-      <c r="B10">
+      <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -544,8 +569,5 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>